<commit_message>
Edits to interpolation method, other bug fixes
</commit_message>
<xml_diff>
--- a/Travis_County/Documentation/Travis_County_2017_bg_config.xlsx
+++ b/Travis_County/Documentation/Travis_County_2017_bg_config.xlsx
@@ -462,7 +462,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['QEXTRCT' 'QHISPC' 'QSERV' 'QEDLESHI' 'PPUNIT' 'QESL' 'QNOHLTH' 'QFHH'
+          <t>['QSERV' 'QESL' 'QNOHLTH' 'QEDLESHI' 'QEXTRCT' 'QHISPC' 'PPUNIT' 'QFHH'
  'PERCAP']</t>
         </is>
       </c>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['MEDAGE' 'QAGEDEP' 'QSSBEN']</t>
+          <t>['QAGEDEP' 'QSSBEN' 'MEDAGE']</t>
         </is>
       </c>
     </row>
@@ -584,67 +584,67 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>QEXTRCT</t>
+          <t>QSERV</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7638644837978544</v>
+        <v>0.5788572269334414</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1521521468101343</v>
+        <v>0.3591286421625365</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01442734711240227</v>
+        <v>-0.2252310192538391</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.2421830645622973</v>
+        <v>-0.03396987931677808</v>
       </c>
       <c r="F2" t="n">
-        <v>0.09804516110051513</v>
+        <v>0.2788530180455505</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>QHISPC</t>
+          <t>QESL</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8302558135818671</v>
+        <v>0.7948904984323639</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3391482222014787</v>
+        <v>0.1613825334468211</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.1355137693461113</v>
+        <v>-0.03005137998308928</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.1303520330212266</v>
+        <v>-0.2422038143621637</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1010584353035389</v>
+        <v>0.2090795683955667</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>QSERV</t>
+          <t>QNOHLTH</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5788572287146556</v>
+        <v>0.6835885831892797</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3591286431006653</v>
+        <v>0.4274092513584713</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.2252310191804674</v>
+        <v>-0.1180986227688646</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.03396987909238718</v>
+        <v>-0.1193419859649904</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2788530186420672</v>
+        <v>0.2783959678079707</v>
       </c>
     </row>
     <row r="5">
@@ -654,85 +654,85 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8742754488476727</v>
+        <v>0.8742754545694222</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2170987418690177</v>
+        <v>0.2170987387450964</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.01552035512869719</v>
+        <v>-0.01552035325745195</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.1115375103406581</v>
+        <v>-0.1115375102429765</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1928903304552343</v>
+        <v>0.1928903334309309</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>PPUNIT</t>
+          <t>QEXTRCT</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7423686855914378</v>
+        <v>0.7638644823218199</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.02716542987573787</v>
+        <v>0.1521521475853751</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.1540540919879387</v>
+        <v>0.01442734521604606</v>
       </c>
       <c r="E6" t="n">
-        <v>0.05737345460886396</v>
+        <v>-0.2421830635724205</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.4605803671083169</v>
+        <v>0.0980451600571053</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>QESL</t>
+          <t>QHISPC</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.7948904941346708</v>
+        <v>0.8302558099045889</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1613825363420291</v>
+        <v>0.3391482215877205</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.03005138076246831</v>
+        <v>-0.1355137705952958</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.2422038132316587</v>
+        <v>-0.1303520320439234</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2090795663808731</v>
+        <v>0.1010584356086445</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>QNOHLTH</t>
+          <t>PPUNIT</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.6835885811258524</v>
+        <v>0.7423686833126053</v>
       </c>
       <c r="C8" t="n">
-        <v>0.4274092505683565</v>
+        <v>-0.02716542760737626</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1180986241044564</v>
+        <v>-0.1540540875389355</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.1193419855234621</v>
+        <v>0.05737345372566562</v>
       </c>
       <c r="F8" t="n">
-        <v>0.2783959649735657</v>
+        <v>-0.4605803611641273</v>
       </c>
     </row>
     <row r="9">
@@ -742,19 +742,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.5649722656923825</v>
+        <v>0.5649722670226905</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2979097568480658</v>
+        <v>0.2979097563303481</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.09661690057832792</v>
+        <v>-0.09661690089936902</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2627433091601559</v>
+        <v>0.2627433105522369</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.02662914661195298</v>
+        <v>-0.02662914703716459</v>
       </c>
     </row>
     <row r="10">
@@ -764,19 +764,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.4913747734747737</v>
+        <v>0.491374773462963</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7088158662515326</v>
+        <v>0.7088158683189665</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.27633328123184</v>
+        <v>-0.276333280934828</v>
       </c>
       <c r="E10" t="n">
-        <v>0.05584477719388864</v>
+        <v>0.05584477791462314</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1848051840538185</v>
+        <v>0.1848051844184266</v>
       </c>
     </row>
     <row r="11">
@@ -786,19 +786,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.2130132767242923</v>
+        <v>0.213013272636517</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8688064454830422</v>
+        <v>0.8688064563089002</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.1838949653093993</v>
+        <v>-0.1838949632965971</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.01368674842551369</v>
+        <v>-0.01368674942245885</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2842078607549136</v>
+        <v>0.2842078608904167</v>
       </c>
     </row>
     <row r="12">
@@ -808,85 +808,85 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3700960055164902</v>
+        <v>0.3700960064485249</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7551164633976762</v>
+        <v>0.7551164634472819</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.01873357720702522</v>
+        <v>-0.0187335771015702</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.01138785938915081</v>
+        <v>-0.01138785929196793</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.01732184961265906</v>
+        <v>-0.01732185127475163</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>MEDAGE</t>
+          <t>QAGEDEP</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.3100329717612146</v>
+        <v>-0.04257251893742132</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.2422549007625328</v>
+        <v>-0.1105675146675588</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7910147369594183</v>
+        <v>0.6577462371544496</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.01282271464150767</v>
+        <v>0.6416531589319452</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.2761421313412767</v>
+        <v>-0.1145417532589742</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>QAGEDEP</t>
+          <t>QSSBEN</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.04257251915313443</v>
+        <v>0.01958181058519956</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.1105675150796839</v>
+        <v>-0.05546784723718445</v>
       </c>
       <c r="D14" t="n">
-        <v>0.6577462321857852</v>
+        <v>0.7724236636677263</v>
       </c>
       <c r="E14" t="n">
-        <v>0.6416531563201519</v>
+        <v>0.1368589223097694</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.1145417548156409</v>
+        <v>-0.1456422712177872</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>QSSBEN</t>
+          <t>MEDAGE</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.01958181138665046</v>
+        <v>-0.310032971999737</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.05546784866896107</v>
+        <v>-0.2422549013545611</v>
       </c>
       <c r="D15" t="n">
-        <v>0.772423657369135</v>
+        <v>0.7910147337033275</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1368589248421451</v>
+        <v>-0.01282271536411952</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.1456422737443327</v>
+        <v>-0.2761421321301501</v>
       </c>
     </row>
     <row r="16">
@@ -896,19 +896,19 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.2392027560440681</v>
+        <v>-0.2392027557165198</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0811548465551714</v>
+        <v>0.08115484564614343</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.02961507276427129</v>
+        <v>-0.02961507201535967</v>
       </c>
       <c r="E16" t="n">
-        <v>0.7870156621266238</v>
+        <v>0.7870156598199922</v>
       </c>
       <c r="F16" t="n">
-        <v>0.002700677519617279</v>
+        <v>0.002700677784901289</v>
       </c>
     </row>
     <row r="17">
@@ -918,19 +918,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.04558114562471189</v>
+        <v>-0.04558114523530072</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.04877177769449419</v>
+        <v>-0.04877177825685924</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1719743037565048</v>
+        <v>0.1719743026450634</v>
       </c>
       <c r="E17" t="n">
-        <v>0.8732591091560415</v>
+        <v>0.8732591131431345</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.02403664882045099</v>
+        <v>-0.02403664950012062</v>
       </c>
     </row>
     <row r="18">
@@ -940,19 +940,19 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.007369445485297376</v>
+        <v>0.007369445308590607</v>
       </c>
       <c r="C18" t="n">
-        <v>0.2404828202505685</v>
+        <v>0.2404828217006364</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.4212014992511496</v>
+        <v>-0.4212014999083357</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.09993109744964952</v>
+        <v>-0.09993109697197729</v>
       </c>
       <c r="F18" t="n">
-        <v>0.7593165793883973</v>
+        <v>0.7593165704367276</v>
       </c>
     </row>
     <row r="19">
@@ -962,19 +962,19 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.3702864796658859</v>
+        <v>0.3702864779202081</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1444159357787117</v>
+        <v>0.1444159373175141</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.3834144481262652</v>
+        <v>-0.3834144468126657</v>
       </c>
       <c r="E19" t="n">
-        <v>0.08162395712160224</v>
+        <v>0.08162395691949784</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4744661423812429</v>
+        <v>0.4744661448571343</v>
       </c>
     </row>
     <row r="20">
@@ -984,19 +984,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1603482010506206</v>
+        <v>0.1603481989507422</v>
       </c>
       <c r="C20" t="n">
-        <v>0.06253916295373532</v>
+        <v>0.06253916239658538</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.1037263537036849</v>
+        <v>-0.1037263512179677</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.01653642123586171</v>
+        <v>-0.01653642180616662</v>
       </c>
       <c r="F20" t="n">
-        <v>0.6401537731055346</v>
+        <v>0.6401537827355265</v>
       </c>
     </row>
   </sheetData>
@@ -1112,55 +1112,55 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.357711898837612</v>
+        <v>5.357711907063933</v>
       </c>
       <c r="C2" t="n">
-        <v>2.502681425536469</v>
+        <v>2.502681462413677</v>
       </c>
       <c r="D2" t="n">
-        <v>2.317329290740203</v>
+        <v>2.317329284213393</v>
       </c>
       <c r="E2" t="n">
-        <v>2.200799343495055</v>
+        <v>2.200799336869337</v>
       </c>
       <c r="F2" t="n">
-        <v>2.006259115701981</v>
+        <v>2.006259110707016</v>
       </c>
       <c r="G2" t="n">
-        <v>1.600413650406493</v>
+        <v>1.600413605322627</v>
       </c>
       <c r="H2" t="n">
-        <v>1.000035941424681</v>
+        <v>1.000035936442935</v>
       </c>
       <c r="I2" t="n">
-        <v>4.773468752227155</v>
+        <v>4.773468753771055</v>
       </c>
       <c r="J2" t="n">
-        <v>3.404064017950268</v>
+        <v>3.404064001175622</v>
       </c>
       <c r="K2" t="n">
-        <v>2.235666409598234</v>
+        <v>2.235666416925869</v>
       </c>
       <c r="L2" t="n">
-        <v>2.054347870397088</v>
+        <v>2.054347870287409</v>
       </c>
       <c r="M2" t="n">
-        <v>2.034144207232764</v>
+        <v>2.034144212558734</v>
       </c>
       <c r="N2" t="n">
-        <v>5.085980807883531</v>
+        <v>5.085980812112077</v>
       </c>
       <c r="O2" t="n">
-        <v>2.605486844222652</v>
+        <v>2.605486864154571</v>
       </c>
       <c r="P2" t="n">
-        <v>2.248589708834145</v>
+        <v>2.248589716232898</v>
       </c>
       <c r="Q2" t="n">
-        <v>2.067416296523605</v>
+        <v>2.067416303071898</v>
       </c>
       <c r="R2" t="n">
-        <v>1.906728079165129</v>
+        <v>1.906728077536314</v>
       </c>
     </row>
     <row r="3">
@@ -1170,55 +1170,55 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1984337740310227</v>
+        <v>0.1984337743357012</v>
       </c>
       <c r="C3" t="n">
-        <v>0.09269190464949884</v>
+        <v>0.09269190601532136</v>
       </c>
       <c r="D3" t="n">
-        <v>0.08582701076815565</v>
+        <v>0.08582701052642197</v>
       </c>
       <c r="E3" t="n">
-        <v>0.08151108679611317</v>
+        <v>0.08151108655071618</v>
       </c>
       <c r="F3" t="n">
-        <v>0.07430589317414746</v>
+        <v>0.07430589298914875</v>
       </c>
       <c r="G3" t="n">
-        <v>0.05927457964468491</v>
+        <v>0.0592745779749121</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0370383682009141</v>
+        <v>0.03703836801640502</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2273080358203407</v>
+        <v>0.2273080358938598</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1620982865690604</v>
+        <v>0.1620982857702677</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1064603052189635</v>
+        <v>0.1064603055678985</v>
       </c>
       <c r="L3" t="n">
-        <v>0.09782608906652801</v>
+        <v>0.09782608906130517</v>
       </c>
       <c r="M3" t="n">
-        <v>0.09686400986822685</v>
+        <v>0.09686401012184448</v>
       </c>
       <c r="N3" t="n">
-        <v>0.2676832004149227</v>
+        <v>0.2676832006374777</v>
       </c>
       <c r="O3" t="n">
-        <v>0.1371308865380343</v>
+        <v>0.1371308875870827</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1183468267807445</v>
+        <v>0.1183468271701525</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.1088113840275582</v>
+        <v>0.1088113843722052</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1003541094297436</v>
+        <v>0.1003541093440165</v>
       </c>
     </row>
     <row r="4">
@@ -1228,55 +1228,55 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1984337740310227</v>
+        <v>0.1984337743357012</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2911256786805215</v>
+        <v>0.2911256803510226</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3769526894486772</v>
+        <v>0.3769526908774445</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4584637762447903</v>
+        <v>0.4584637774281607</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5327696694189378</v>
+        <v>0.5327696704173095</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5920442490636226</v>
+        <v>0.5920442483922216</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6290826172645367</v>
+        <v>0.6290826164086266</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2273080358203407</v>
+        <v>0.2273080358938598</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3894063223894011</v>
+        <v>0.3894063216641275</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4958666276083646</v>
+        <v>0.495866627232026</v>
       </c>
       <c r="L4" t="n">
-        <v>0.5936927166748927</v>
+        <v>0.5936927162933312</v>
       </c>
       <c r="M4" t="n">
-        <v>0.6905567265431195</v>
+        <v>0.6905567264151757</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2676832004149227</v>
+        <v>0.2676832006374777</v>
       </c>
       <c r="O4" t="n">
-        <v>0.404814086952957</v>
+        <v>0.4048140882245604</v>
       </c>
       <c r="P4" t="n">
-        <v>0.5231609137337014</v>
+        <v>0.523160915394713</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.6319722977612596</v>
+        <v>0.6319722997669182</v>
       </c>
       <c r="R4" t="n">
-        <v>0.7323264071910033</v>
+        <v>0.7323264091109347</v>
       </c>
     </row>
     <row r="5">
@@ -1286,55 +1286,55 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.3154335672059731</v>
+        <v>0.3154335681194641</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1473445650947319</v>
+        <v>0.1473445674663381</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1364320176916673</v>
+        <v>0.1364320174930286</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1295713544757457</v>
+        <v>0.1295713542619494</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1181178610486084</v>
+        <v>0.1181178609152389</v>
       </c>
       <c r="G5" t="n">
-        <v>0.09422383963243296</v>
+        <v>0.09422383710633285</v>
       </c>
       <c r="H5" t="n">
-        <v>0.05887679485084076</v>
+        <v>0.05887679463764803</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3291663480829872</v>
+        <v>0.3291663482504374</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2347356565195064</v>
+        <v>0.23473565540626</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1541659086457627</v>
+        <v>0.1541659091796212</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1416626401660568</v>
+        <v>0.1416626401847403</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1402694465856868</v>
+        <v>0.1402694469789409</v>
       </c>
       <c r="N5" t="n">
-        <v>0.3655244407226548</v>
+        <v>0.3655244400682652</v>
       </c>
       <c r="O5" t="n">
-        <v>0.1872537780851432</v>
+        <v>0.1872537790267096</v>
       </c>
       <c r="P5" t="n">
-        <v>0.1616039318241839</v>
+        <v>0.16160393193225</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.1485831767898796</v>
+        <v>0.1485831768709602</v>
       </c>
       <c r="R5" t="n">
-        <v>0.1370346725781385</v>
+        <v>0.137034672101815</v>
       </c>
     </row>
   </sheetData>
@@ -1390,19 +1390,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.085980807883531</v>
+        <v>5.085980812112077</v>
       </c>
       <c r="C2" t="n">
-        <v>2.605486844222652</v>
+        <v>2.605486864154571</v>
       </c>
       <c r="D2" t="n">
-        <v>2.248589708834145</v>
+        <v>2.248589716232898</v>
       </c>
       <c r="E2" t="n">
-        <v>2.067416296523605</v>
+        <v>2.067416303071898</v>
       </c>
       <c r="F2" t="n">
-        <v>1.906728079165129</v>
+        <v>1.906728077536314</v>
       </c>
     </row>
     <row r="3">
@@ -1412,19 +1412,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2676832004149227</v>
+        <v>0.2676832006374777</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1371308865380343</v>
+        <v>0.1371308875870827</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1183468267807445</v>
+        <v>0.1183468271701525</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1088113840275582</v>
+        <v>0.1088113843722052</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1003541094297436</v>
+        <v>0.1003541093440165</v>
       </c>
     </row>
     <row r="4">
@@ -1434,19 +1434,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2676832004149227</v>
+        <v>0.2676832006374777</v>
       </c>
       <c r="C4" t="n">
-        <v>0.404814086952957</v>
+        <v>0.4048140882245604</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5231609137337014</v>
+        <v>0.523160915394713</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6319722977612596</v>
+        <v>0.6319722997669182</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7323264071910033</v>
+        <v>0.7323264091109347</v>
       </c>
     </row>
     <row r="5">
@@ -1456,19 +1456,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.3655244407226548</v>
+        <v>0.3655244400682652</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1872537780851432</v>
+        <v>0.1872537790267096</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1616039318241839</v>
+        <v>0.16160393193225</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1485831767898796</v>
+        <v>0.1485831768709602</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1370346725781385</v>
+        <v>0.137034672101815</v>
       </c>
     </row>
   </sheetData>
@@ -1508,7 +1508,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[['QEXTRCT', 'QHISPC', 'QSERV', 'QEDLESHI', 'PPUNIT', 'QESL', 'QNOHLTH', 'QFHH', 'PERCAP', 'QRICH', 'MDHSEVAL', 'MEDAGE', 'QAGEDEP', 'QSSBEN', 'QFEMLBR', 'QFEMALE', 'QRENTER', 'QPOVTY', 'QNOAUTO']]</t>
+          <t>[['QSERV', 'QESL', 'QNOHLTH', 'QEDLESHI', 'QEXTRCT', 'QHISPC', 'PPUNIT', 'QFHH', 'PERCAP', 'QRICH', 'MDHSEVAL', 'QAGEDEP', 'QSSBEN', 'MEDAGE', 'QFEMLBR', 'QFEMALE', 'QRENTER', 'QPOVTY', 'QNOAUTO']]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">

</xml_diff>